<commit_message>
feat: started pp.runpp() but not converging
</commit_message>
<xml_diff>
--- a/code/Modified_116_LV_CSV/Loads.xlsx
+++ b/code/Modified_116_LV_CSV/Loads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariumkhn\Google Drive\PhD-2020\IEEE_Letter\Modified.116_LV_Test_Feeder\Modified.116_LV_CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96dd476106d6c447/IST Mestrado/Tese Mestrado/DEV/code/Modified_116_LV_CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433E53D5-B6F5-44D6-8B16-8D41B403265A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{433E53D5-B6F5-44D6-8B16-8D41B403265A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F40303C-0D59-400D-BA5C-DC3C5AB7BAEC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,6 +409,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,7 +443,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,7 +727,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +790,7 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>5</v>
       </c>
       <c r="D4" t="s">
@@ -819,7 +822,7 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>7</v>
       </c>
       <c r="D5" t="s">
@@ -851,7 +854,7 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>10</v>
       </c>
       <c r="D6" t="s">
@@ -883,7 +886,7 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>11</v>
       </c>
       <c r="D7" t="s">
@@ -915,7 +918,7 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>12</v>
       </c>
       <c r="D8" t="s">
@@ -947,7 +950,7 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>13</v>
       </c>
       <c r="D9" t="s">
@@ -979,7 +982,7 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>21</v>
       </c>
       <c r="D10" t="s">
@@ -1011,7 +1014,7 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>25</v>
       </c>
       <c r="D11" t="s">
@@ -1043,7 +1046,7 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>26</v>
       </c>
       <c r="D12" t="s">

</xml_diff>

<commit_message>
feat: milestone - 1st runpp_3ph without error
</commit_message>
<xml_diff>
--- a/code/Modified_116_LV_CSV/Loads.xlsx
+++ b/code/Modified_116_LV_CSV/Loads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96dd476106d6c447/IST Mestrado/Tese Mestrado/DEV/code/Modified_116_LV_CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{433E53D5-B6F5-44D6-8B16-8D41B403265A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F40303C-0D59-400D-BA5C-DC3C5AB7BAEC}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{433E53D5-B6F5-44D6-8B16-8D41B403265A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEEC933D-CEA6-4665-9D8A-3F104D0D19D3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="1176" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,8 +412,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -441,9 +449,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,7 +736,7 @@
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,7 +1701,7 @@
       <c r="D32" t="s">
         <v>67</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>0.23</v>
       </c>
       <c r="F32">

</xml_diff>